<commit_message>
Updating Algorithms and advanced Checking
- Get new ProposedPreprocessing XLSX
- Adjust Plotting and Cutting offf
- Additional Comments
</commit_message>
<xml_diff>
--- a/src/data_preprocessing/ProposedProcessing.xlsx
+++ b/src/data_preprocessing/ProposedProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barak\Documents\GitHub\MindEyeV2EEG\src\data_preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7F8DA8-EB94-489A-A092-139D77340C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06648287-A39C-44C8-B5D1-9393AFE13257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7F765090-FB2C-43F8-8334-F50482A6F18D}"/>
   </bookViews>
@@ -561,7 +561,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,16 +591,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1000</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -625,16 +625,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>250</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -642,16 +642,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>250</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -676,16 +676,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>100</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -693,16 +693,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>1000</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -727,16 +727,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>250</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -744,16 +744,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>250</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -761,16 +761,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>100</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -778,16 +778,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>100</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="5" t="s">

</xml_diff>